<commit_message>
added shortlinks to task book
</commit_message>
<xml_diff>
--- a/Block01-Methodologie/Live-Experiment-Regression_to_the_mean.xlsx
+++ b/Block01-Methodologie/Live-Experiment-Regression_to_the_mean.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samuelmerk/Nextcloud/Lehre/Lehre_WS_2425/VL-Forschungsmethoden-WiSe2425/Block01-Methodologie/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0AE5E84-F57D-6B4A-A5D6-130F0D336774}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB10AC86-CDE6-644A-81DB-0428C486537D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3840" yWindow="500" windowWidth="34560" windowHeight="21100" xr2:uid="{A0494C58-B0C1-5A42-BA17-0C7F278390D5}"/>
+    <workbookView xWindow="0" yWindow="1000" windowWidth="34560" windowHeight="21100" xr2:uid="{A0494C58-B0C1-5A42-BA17-0C7F278390D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -89,12 +90,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="7">
@@ -171,7 +178,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -186,6 +193,9 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -503,7 +513,7 @@
   <dimension ref="A1:I102"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="217" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A18"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -530,32 +540,37 @@
     </row>
     <row r="2" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="str">
         <f t="shared" ref="B2:B65" si="0">IF(A1="","",IF(A1=1, "JA",IF(A1=2,"JA","NEIN")))</f>
         <v>NEIN</v>
       </c>
+      <c r="C2" s="10" t="str">
+        <f>IF(B2="NEIN","",A2-A1)</f>
+        <v/>
+      </c>
+      <c r="D2" s="10"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>JA</v>
-      </c>
-      <c r="C3" s="1">
-        <f>IF(B3="JA",A3-A2,"")</f>
-        <v>3</v>
-      </c>
-      <c r="D3" s="1" t="str">
-        <f>IF(B3="NEIN",A3-A2,"")</f>
-        <v/>
+        <v>NEIN</v>
+      </c>
+      <c r="C3" s="1" t="str">
+        <f t="shared" ref="C3:C17" si="1">IF(B3="NEIN","",A3-A2)</f>
+        <v/>
+      </c>
+      <c r="D3" s="1">
+        <f t="shared" ref="D3:D17" si="2">IF(B3="NEIN",A3-A2,"")</f>
+        <v>2</v>
       </c>
       <c r="E3" s="4">
         <f>AVERAGE(C3:C200)</f>
-        <v>2.4</v>
+        <v>2.6666666666666665</v>
       </c>
       <c r="F3" s="5" t="s">
         <v>5</v>
@@ -566,23 +581,23 @@
     </row>
     <row r="4" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1" t="str">
         <f t="shared" si="0"/>
         <v>NEIN</v>
       </c>
       <c r="C4" s="1" t="str">
-        <f t="shared" ref="C4:C67" si="1">IF(B4="JA",A4-A3,"")</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="D4" s="1">
-        <f t="shared" ref="D4:D67" si="2">IF(B4="NEIN",A4-A3,"")</f>
-        <v>-1</v>
+        <f t="shared" si="2"/>
+        <v>1</v>
       </c>
       <c r="E4" s="7">
         <f>AVERAGE(D3:D200)</f>
-        <v>-1.0833333333333333</v>
+        <v>-0.58333333333333337</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>4</v>
@@ -605,12 +620,12 @@
       </c>
       <c r="D5" s="1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1" t="str">
         <f t="shared" si="0"/>
@@ -622,46 +637,46 @@
       </c>
       <c r="D6" s="1">
         <f t="shared" si="2"/>
-        <v>-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B7" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>JA</v>
-      </c>
-      <c r="C7" s="1">
+        <v>NEIN</v>
+      </c>
+      <c r="C7" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="D7" s="1" t="str">
+        <v/>
+      </c>
+      <c r="D7" s="1">
         <f t="shared" si="2"/>
-        <v/>
+        <v>-3</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>NEIN</v>
-      </c>
-      <c r="C8" s="1" t="str">
+        <v>JA</v>
+      </c>
+      <c r="C8" s="1">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="D8" s="1">
+        <v>5</v>
+      </c>
+      <c r="D8" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v/>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B9" s="1" t="str">
         <f t="shared" si="0"/>
@@ -673,41 +688,41 @@
       </c>
       <c r="D9" s="1">
         <f t="shared" si="2"/>
-        <v>-2</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B10" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>JA</v>
-      </c>
-      <c r="C10" s="1">
+        <v>NEIN</v>
+      </c>
+      <c r="C10" s="1" t="str">
         <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="D10" s="1">
+        <f t="shared" si="2"/>
         <v>1</v>
-      </c>
-      <c r="D10" s="1" t="str">
-        <f t="shared" si="2"/>
-        <v/>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B11" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>JA</v>
-      </c>
-      <c r="C11" s="1">
+        <v>NEIN</v>
+      </c>
+      <c r="C11" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="D11" s="1" t="str">
+        <v/>
+      </c>
+      <c r="D11" s="1">
         <f t="shared" si="2"/>
-        <v/>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -724,12 +739,12 @@
       </c>
       <c r="D12" s="1">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B13" s="1" t="str">
         <f t="shared" si="0"/>
@@ -741,58 +756,58 @@
       </c>
       <c r="D13" s="1">
         <f t="shared" si="2"/>
-        <v>-2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B14" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>JA</v>
-      </c>
-      <c r="C14" s="1">
+        <v>NEIN</v>
+      </c>
+      <c r="C14" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="D14" s="1" t="str">
+        <v/>
+      </c>
+      <c r="D14" s="1">
         <f t="shared" si="2"/>
-        <v/>
+        <v>-5</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B15" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>NEIN</v>
-      </c>
-      <c r="C15" s="1" t="str">
+        <v>JA</v>
+      </c>
+      <c r="C15" s="1">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="D15" s="1">
+        <v>1</v>
+      </c>
+      <c r="D15" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v/>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B16" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>NEIN</v>
-      </c>
-      <c r="C16" s="1" t="str">
+        <v>JA</v>
+      </c>
+      <c r="C16" s="1">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="D16" s="1">
+        <v>2</v>
+      </c>
+      <c r="D16" s="1" t="str">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v/>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -809,38 +824,19 @@
       </c>
       <c r="D17" s="1">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="1">
-        <v>3</v>
-      </c>
       <c r="B18" s="1" t="str">
         <f t="shared" si="0"/>
         <v>NEIN</v>
-      </c>
-      <c r="C18" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="D18" s="1">
-        <f t="shared" si="2"/>
-        <v>-1</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>NEIN</v>
-      </c>
-      <c r="C19" s="1" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="D19" s="1">
-        <f t="shared" si="2"/>
-        <v>-3</v>
+        <v/>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -849,11 +845,11 @@
         <v/>
       </c>
       <c r="C20" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="C4:C67" si="3">IF(B20="JA",A20-A19,"")</f>
         <v/>
       </c>
       <c r="D20" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="D4:D67" si="4">IF(B20="NEIN",A20-A19,"")</f>
         <v/>
       </c>
     </row>
@@ -863,11 +859,11 @@
         <v/>
       </c>
       <c r="C21" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D21" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -877,11 +873,11 @@
         <v/>
       </c>
       <c r="C22" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D22" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -891,11 +887,11 @@
         <v/>
       </c>
       <c r="C23" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D23" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -905,11 +901,11 @@
         <v/>
       </c>
       <c r="C24" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D24" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -919,11 +915,11 @@
         <v/>
       </c>
       <c r="C25" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D25" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -933,11 +929,11 @@
         <v/>
       </c>
       <c r="C26" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D26" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -947,11 +943,11 @@
         <v/>
       </c>
       <c r="C27" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D27" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -961,11 +957,11 @@
         <v/>
       </c>
       <c r="C28" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D28" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -975,11 +971,11 @@
         <v/>
       </c>
       <c r="C29" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D29" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -989,11 +985,11 @@
         <v/>
       </c>
       <c r="C30" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D30" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -1003,11 +999,11 @@
         <v/>
       </c>
       <c r="C31" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D31" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -1017,11 +1013,11 @@
         <v/>
       </c>
       <c r="C32" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D32" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -1031,11 +1027,11 @@
         <v/>
       </c>
       <c r="C33" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D33" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -1045,11 +1041,11 @@
         <v/>
       </c>
       <c r="C34" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D34" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -1059,11 +1055,11 @@
         <v/>
       </c>
       <c r="C35" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D35" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -1073,11 +1069,11 @@
         <v/>
       </c>
       <c r="C36" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D36" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -1087,11 +1083,11 @@
         <v/>
       </c>
       <c r="C37" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D37" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -1101,11 +1097,11 @@
         <v/>
       </c>
       <c r="C38" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D38" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -1115,11 +1111,11 @@
         <v/>
       </c>
       <c r="C39" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D39" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -1129,11 +1125,11 @@
         <v/>
       </c>
       <c r="C40" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D40" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -1143,11 +1139,11 @@
         <v/>
       </c>
       <c r="C41" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D41" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -1157,11 +1153,11 @@
         <v/>
       </c>
       <c r="C42" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D42" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -1171,11 +1167,11 @@
         <v/>
       </c>
       <c r="C43" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D43" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -1185,11 +1181,11 @@
         <v/>
       </c>
       <c r="C44" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D44" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -1199,11 +1195,11 @@
         <v/>
       </c>
       <c r="C45" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D45" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -1213,11 +1209,11 @@
         <v/>
       </c>
       <c r="C46" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D46" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -1227,11 +1223,11 @@
         <v/>
       </c>
       <c r="C47" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D47" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -1241,11 +1237,11 @@
         <v/>
       </c>
       <c r="C48" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D48" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -1255,11 +1251,11 @@
         <v/>
       </c>
       <c r="C49" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D49" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -1269,11 +1265,11 @@
         <v/>
       </c>
       <c r="C50" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D50" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -1283,11 +1279,11 @@
         <v/>
       </c>
       <c r="C51" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D51" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -1297,11 +1293,11 @@
         <v/>
       </c>
       <c r="C52" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D52" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -1311,11 +1307,11 @@
         <v/>
       </c>
       <c r="C53" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D53" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -1325,11 +1321,11 @@
         <v/>
       </c>
       <c r="C54" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D54" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -1339,11 +1335,11 @@
         <v/>
       </c>
       <c r="C55" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D55" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -1353,11 +1349,11 @@
         <v/>
       </c>
       <c r="C56" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D56" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -1367,11 +1363,11 @@
         <v/>
       </c>
       <c r="C57" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D57" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -1381,11 +1377,11 @@
         <v/>
       </c>
       <c r="C58" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D58" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -1395,11 +1391,11 @@
         <v/>
       </c>
       <c r="C59" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D59" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -1409,11 +1405,11 @@
         <v/>
       </c>
       <c r="C60" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D60" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -1423,11 +1419,11 @@
         <v/>
       </c>
       <c r="C61" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D61" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -1437,11 +1433,11 @@
         <v/>
       </c>
       <c r="C62" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D62" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -1451,11 +1447,11 @@
         <v/>
       </c>
       <c r="C63" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D63" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -1465,11 +1461,11 @@
         <v/>
       </c>
       <c r="C64" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D64" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -1479,533 +1475,545 @@
         <v/>
       </c>
       <c r="C65" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D65" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B66" s="1" t="str">
-        <f t="shared" ref="B66:B102" si="3">IF(A65="","",IF(A65=1, "JA",IF(A65=2,"JA","NEIN")))</f>
+        <f t="shared" ref="B66:B102" si="5">IF(A65="","",IF(A65=1, "JA",IF(A65=2,"JA","NEIN")))</f>
         <v/>
       </c>
       <c r="C66" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D66" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B67" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C67" s="1" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="D67" s="1" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
     <row r="68" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B68" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C68" s="1" t="str">
-        <f t="shared" ref="C68:C102" si="4">IF(B68="JA",A68-A67,"")</f>
+        <f t="shared" ref="C68:C102" si="6">IF(B68="JA",A68-A67,"")</f>
         <v/>
       </c>
       <c r="D68" s="1" t="str">
-        <f t="shared" ref="D68:D102" si="5">IF(B68="NEIN",A68-A67,"")</f>
+        <f t="shared" ref="D68:D102" si="7">IF(B68="NEIN",A68-A67,"")</f>
         <v/>
       </c>
     </row>
     <row r="69" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B69" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C69" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="D69" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="70" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B70" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C70" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="D70" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="71" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B71" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C71" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="D71" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="72" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B72" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C72" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="D72" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="73" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B73" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C73" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="D73" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="74" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B74" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C74" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="D74" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="75" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B75" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C75" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="D75" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="76" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B76" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C76" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="D76" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="77" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B77" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C77" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="D77" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="78" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B78" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C78" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="D78" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="79" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B79" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C79" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="D79" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="80" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B80" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C80" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="D80" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="81" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B81" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C81" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="D81" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="82" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B82" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C82" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="D82" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="83" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B83" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C83" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="D83" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="84" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B84" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C84" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="D84" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="85" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B85" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C85" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="D85" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="86" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B86" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C86" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="D86" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="87" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B87" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C87" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="D87" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="88" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B88" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C88" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="D88" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="89" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B89" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C89" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="D89" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="90" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B90" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C90" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="D90" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="91" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B91" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C91" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="D91" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="92" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B92" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C92" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="D92" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="93" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B93" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C93" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="D93" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="94" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B94" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C94" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="D94" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="95" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B95" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C95" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="D95" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="96" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B96" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C96" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="D96" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="97" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B97" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C97" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="D97" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="98" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B98" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C98" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="D98" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="99" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B99" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C99" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="D99" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="100" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B100" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C100" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="D100" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="101" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B101" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C101" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="D101" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
     <row r="102" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B102" s="1" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="C102" s="1" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="D102" s="1" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="7"/>
         <v/>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6CC68E4-BA4E-694A-A328-E67BA1B40D2A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView zoomScale="150" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>